<commit_message>
push latest to merge with 4.0
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
@@ -14,12 +14,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
   <si>
+    <t>Supported Browser Types</t>
+  </si>
+  <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
     <t>MozillaFirefox</t>
   </si>
   <si>
@@ -242,7 +242,7 @@
     <t>ImpersonationMessage</t>
   </si>
   <si>
-    <t>You’re temporarily logged in as Analyzer User. To switch back to your account, click on the icon at the bottom left of your screen.</t>
+    <t>You’re temporarily logged in as Analyzer User.</t>
   </si>
   <si>
     <t>Schedule Schema Incremental load</t>
@@ -403,7 +403,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -3623,7 +3623,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>

</xml_diff>

<commit_message>
switch to iframe & switch to default
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
@@ -12,12 +12,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
+  <si>
+    <t>Variable</t>
+  </si>
   <si>
     <t>Supported Browser Types</t>
   </si>
   <si>
-    <t>Variable</t>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>Data5</t>
+  </si>
+  <si>
+    <t>Data6</t>
+  </si>
+  <si>
+    <t>Data7</t>
+  </si>
+  <si>
+    <t>Data8</t>
+  </si>
+  <si>
+    <t>Data9</t>
   </si>
   <si>
     <t>MozillaFirefox</t>
@@ -32,33 +59,6 @@
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
-  <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>Data5</t>
-  </si>
-  <si>
-    <t>Data6</t>
-  </si>
-  <si>
-    <t>Data7</t>
-  </si>
-  <si>
-    <t>Data8</t>
-  </si>
-  <si>
-    <t>Data9</t>
-  </si>
-  <si>
     <t>URLs</t>
   </si>
   <si>
@@ -77,49 +77,46 @@
     <t>URL_content_allContent</t>
   </si>
   <si>
-    <t>#/all-content</t>
-  </si>
-  <si>
     <t>URL_security_groups</t>
   </si>
   <si>
-    <t>#/security/groups</t>
+    <t>new/~/security/groups</t>
   </si>
   <si>
     <t>URL_security_users</t>
   </si>
   <si>
-    <t>#/security/users</t>
+    <t>new/~/security/users</t>
   </si>
   <si>
     <t>URL_data_dataSources</t>
   </si>
   <si>
-    <t>#/datasources/datasource</t>
+    <t>new/~/datasources/datasource</t>
   </si>
   <si>
     <t>URL_data_dataFiles</t>
   </si>
   <si>
-    <t>#/datasources/dataFiles</t>
+    <t>new/~/datasources/dataFiles</t>
   </si>
   <si>
     <t>URL_schemas_schemaList</t>
   </si>
   <si>
-    <t>#/schemas/schema-list</t>
+    <t>new/~/schemas/schema-list</t>
   </si>
   <si>
     <t>URL_scheduler_schemas</t>
   </si>
   <si>
-    <t>#/schedulers/scheduler-schemas</t>
+    <t>new/~/schedulers/scheduler-schemas</t>
   </si>
   <si>
     <t>URL_scheduler_dashboards</t>
   </si>
   <si>
-    <t>#/schedulers/scheduler-dashboards</t>
+    <t>new/~/schedulers/scheduler-dashboards</t>
   </si>
   <si>
     <t>User Credentials Analyzer</t>
@@ -335,11 +332,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -402,35 +399,35 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -546,7 +543,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -575,10 +572,10 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -607,10 +604,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -639,10 +636,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -671,10 +668,10 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -703,10 +700,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -735,10 +732,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -767,10 +764,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -799,7 +796,7 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -827,34 +824,34 @@
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="C14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -875,34 +872,34 @@
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="I15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="J15" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
@@ -923,34 +920,34 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="H16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="I16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="J16" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
@@ -971,7 +968,7 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -999,13 +996,13 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -1033,13 +1030,13 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1067,13 +1064,13 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -1101,13 +1098,13 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="C21" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -1135,13 +1132,13 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -1169,7 +1166,7 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1197,13 +1194,13 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -1231,13 +1228,13 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="C25" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -1265,7 +1262,7 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1293,13 +1290,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -1327,7 +1324,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1355,10 +1352,10 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1387,10 +1384,10 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="4"/>
@@ -1419,7 +1416,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -1447,7 +1444,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -1477,10 +1474,10 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -1509,10 +1506,10 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -1541,10 +1538,10 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -1573,10 +1570,10 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1605,10 +1602,10 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -3622,79 +3619,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Updated the below: TC 14,2,3 Are failing due to IFrame Issue. Even after switching to non IFrame web page, it’s still failing. =------------=------------=------------ TC 4 Is failing due to an issue in “Please load data from QA side”. Waiting for the fix. =------------=------------=------------ TC 5 Passed =------------=------------=------------ TC6 Need to correct last step in the assertion that user cannot share - But there’s a defect In this step - So It will be checked after it’s fixed. subHeaderObject.assertExportIconIsNotDisplayed(); dashboardPage.assert_shared_button_dimmed(); =------------=------------=------------ TestData - Updated with new URLs.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
@@ -14,15 +14,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
   <si>
+    <t>Supported Browser Types</t>
+  </si>
+  <si>
     <t>Variable</t>
   </si>
   <si>
-    <t>Supported Browser Types</t>
-  </si>
-  <si>
     <t>Data1</t>
   </si>
   <si>
+    <t>MozillaFirefox</t>
+  </si>
+  <si>
     <t>Data2</t>
   </si>
   <si>
@@ -47,31 +50,28 @@
     <t>Data9</t>
   </si>
   <si>
-    <t>MozillaFirefox</t>
-  </si>
-  <si>
     <t>GoogleChrome</t>
   </si>
   <si>
     <t>MicrosoftInternetExplorer</t>
   </si>
   <si>
+    <t>URLs</t>
+  </si>
+  <si>
     <t>MicrosoftEdge</t>
   </si>
   <si>
-    <t>URLs</t>
-  </si>
-  <si>
     <t>URL_login_login</t>
   </si>
   <si>
-    <t>new/login</t>
+    <t>#/login</t>
   </si>
   <si>
     <t>URL_content</t>
   </si>
   <si>
-    <t>new/catalog</t>
+    <t>#/catalog</t>
   </si>
   <si>
     <t>URL_content_allContent</t>
@@ -80,43 +80,43 @@
     <t>URL_security_groups</t>
   </si>
   <si>
-    <t>new/~/security/groups</t>
+    <t>#/~/security/groups</t>
   </si>
   <si>
     <t>URL_security_users</t>
   </si>
   <si>
-    <t>new/~/security/users</t>
+    <t>#/~/security/users</t>
   </si>
   <si>
     <t>URL_data_dataSources</t>
   </si>
   <si>
-    <t>new/~/datasources/datasource</t>
+    <t>#/~/datasources/datasource</t>
   </si>
   <si>
     <t>URL_data_dataFiles</t>
   </si>
   <si>
-    <t>new/~/datasources/dataFiles</t>
+    <t>#/~/datasources/dataFiles</t>
   </si>
   <si>
     <t>URL_schemas_schemaList</t>
   </si>
   <si>
-    <t>new/~/schemas/schema-list</t>
+    <t>#/~/schemas/schema-list</t>
   </si>
   <si>
     <t>URL_scheduler_schemas</t>
   </si>
   <si>
-    <t>new/~/schedulers/scheduler-schemas</t>
+    <t>#/~/schedulers/scheduler-schemas</t>
   </si>
   <si>
     <t>URL_scheduler_dashboards</t>
   </si>
   <si>
-    <t>new/~/schedulers/scheduler-dashboards</t>
+    <t>#/~/schedulers/scheduler-dashboards</t>
   </si>
   <si>
     <t>User Credentials Analyzer</t>
@@ -332,11 +332,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -345,9 +345,12 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -357,9 +360,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -399,35 +399,35 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -448,7 +448,7 @@
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -478,22 +478,22 @@
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -510,22 +510,22 @@
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -542,22 +542,22 @@
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -574,22 +574,22 @@
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -606,22 +606,22 @@
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -638,22 +638,22 @@
       <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -670,22 +670,22 @@
       <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -702,22 +702,22 @@
       <c r="A10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -734,22 +734,22 @@
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
@@ -766,22 +766,22 @@
       <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
@@ -853,11 +853,11 @@
       <c r="J14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -901,11 +901,11 @@
       <c r="J15" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
@@ -949,11 +949,11 @@
       <c r="J16" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
@@ -1004,18 +1004,18 @@
       <c r="C18" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
@@ -1032,24 +1032,24 @@
       <c r="A19" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
@@ -1063,27 +1063,27 @@
       <c r="Z19" s="4"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
@@ -1106,18 +1106,18 @@
       <c r="C21" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
@@ -1131,27 +1131,27 @@
       <c r="Z21" s="4"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
@@ -1193,27 +1193,27 @@
       <c r="Z23" s="4"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
@@ -1236,18 +1236,18 @@
       <c r="C25" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
@@ -1298,18 +1298,18 @@
       <c r="C27" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
@@ -1354,7 +1354,7 @@
       <c r="A29" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C29" s="4"/>
@@ -1383,13 +1383,13 @@
       <c r="Z29" s="4"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1443,23 +1443,23 @@
       <c r="Z31" s="4"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -1479,19 +1479,19 @@
       <c r="B33" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
@@ -1511,19 +1511,19 @@
       <c r="B34" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
@@ -1543,19 +1543,19 @@
       <c r="B35" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
@@ -1569,10 +1569,10 @@
       <c r="Z35" s="4"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="4"/>
@@ -1601,10 +1601,10 @@
       <c r="Z36" s="4"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="10" t="s">
         <v>87</v>
       </c>
       <c r="C37" s="4"/>
@@ -1633,8 +1633,8 @@
       <c r="Z37" s="4"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -1661,8 +1661,8 @@
       <c r="Z38" s="4"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -1689,8 +1689,8 @@
       <c r="Z39" s="4"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -1717,8 +1717,8 @@
       <c r="Z40" s="4"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -1745,8 +1745,8 @@
       <c r="Z41" s="4"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -1773,8 +1773,8 @@
       <c r="Z42" s="4"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -1801,8 +1801,8 @@
       <c r="Z43" s="4"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -1829,8 +1829,8 @@
       <c r="Z44" s="4"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -1857,8 +1857,8 @@
       <c r="Z45" s="4"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -1885,8 +1885,8 @@
       <c r="Z46" s="4"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -1913,8 +1913,8 @@
       <c r="Z47" s="4"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -1941,8 +1941,8 @@
       <c r="Z48" s="4"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -1969,8 +1969,8 @@
       <c r="Z49" s="4"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -1997,8 +1997,8 @@
       <c r="Z50" s="4"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -2025,8 +2025,8 @@
       <c r="Z51" s="4"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -2053,8 +2053,8 @@
       <c r="Z52" s="4"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -2081,8 +2081,8 @@
       <c r="Z53" s="4"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -2109,8 +2109,8 @@
       <c r="Z54" s="4"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -2137,8 +2137,8 @@
       <c r="Z55" s="4"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -2165,8 +2165,8 @@
       <c r="Z56" s="4"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -2193,8 +2193,8 @@
       <c r="Z57" s="4"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -2221,8 +2221,8 @@
       <c r="Z58" s="4"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="8"/>
-      <c r="B59" s="10"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -2249,8 +2249,8 @@
       <c r="Z59" s="4"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="8"/>
-      <c r="B60" s="10"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -2277,8 +2277,8 @@
       <c r="Z60" s="4"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="8"/>
-      <c r="B61" s="10"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -2305,8 +2305,8 @@
       <c r="Z61" s="4"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -2333,8 +2333,8 @@
       <c r="Z62" s="4"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -2361,8 +2361,8 @@
       <c r="Z63" s="4"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="10"/>
-      <c r="B64" s="10"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -2389,8 +2389,8 @@
       <c r="Z64" s="4"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="10"/>
-      <c r="B65" s="10"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -2613,8 +2613,8 @@
       <c r="Z72" s="4"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="8"/>
-      <c r="B73" s="8"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -2641,7 +2641,7 @@
       <c r="Z73" s="4"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="8"/>
+      <c r="A74" s="9"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -3587,6 +3587,13 @@
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A2:C2"/>
@@ -3619,79 +3626,79 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
add new test data to data file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFarid\git\qa\src\test\resources\TestDataFiles\security_newUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6364790F-0355-40BF-9A39-2FF239993682}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A6D6B9-E827-4804-B6D9-5BFD96264574}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
   <si>
     <t>Variable</t>
   </si>
@@ -299,6 +299,12 @@
   </si>
   <si>
     <t>.*You can use the link below to sign back in.*</t>
+  </si>
+  <si>
+    <t>Data10</t>
+  </si>
+  <si>
+    <t>Automation_User_SuperUser4</t>
   </si>
 </sst>
 </file>
@@ -364,9 +370,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,6 +380,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,1254 +779,1265 @@
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="6" width="28.28515625" customWidth="1"/>
     <col min="7" max="7" width="28.85546875" customWidth="1"/>
-    <col min="8" max="15" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" customWidth="1"/>
+    <col min="10" max="10" width="28.85546875" customWidth="1"/>
+    <col min="11" max="15" width="8.5703125" customWidth="1"/>
     <col min="16" max="17" width="8.7109375" customWidth="1"/>
     <col min="18" max="1025" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="K1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
+      <c r="K13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
+      <c r="K14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
+      <c r="K15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-      <c r="Z24" s="4"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-      <c r="X28" s="4"/>
-      <c r="Y28" s="4"/>
-      <c r="Z28" s="4"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-      <c r="Z30" s="4"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="4"/>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
-      <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-      <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-      <c r="X36" s="4"/>
-      <c r="Y36" s="4"/>
-      <c r="Z36" s="4"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -3029,79 +3046,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update one testcase in users test class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFarid\git\qa\src\test\resources\TestDataFiles\security_newUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A6D6B9-E827-4804-B6D9-5BFD96264574}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A5E56F-011E-43C5-8200-EF6C25EABD8F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
   <si>
     <t>Variable</t>
   </si>
@@ -305,6 +305,30 @@
   </si>
   <si>
     <t>Automation_User_SuperUser4</t>
+  </si>
+  <si>
+    <t>Automation_Schema_Transfer_Ownership</t>
+  </si>
+  <si>
+    <t>newSchemaName</t>
+  </si>
+  <si>
+    <t>newDashboardName</t>
+  </si>
+  <si>
+    <t>Automation_Dashboard_Transfer_Ownership</t>
+  </si>
+  <si>
+    <t>newFolderName</t>
+  </si>
+  <si>
+    <t>Automation_Folder_Transfer_Ownership</t>
+  </si>
+  <si>
+    <t>Automation_insight_Transfer_Ownership</t>
+  </si>
+  <si>
+    <t>newInsightName</t>
   </si>
 </sst>
 </file>
@@ -765,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1048576"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,27 +2063,178 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+    </row>
+    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+    </row>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+    </row>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="3"/>
+      <c r="Y41" s="3"/>
+      <c r="Z41" s="3"/>
+    </row>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+    </row>
+    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>87</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B43" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="44" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>89</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B44" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3015,17 +3190,23 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A42:C42"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
update security module last test case  also some update.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/security_newUI/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFarid\git\qa\src\test\resources\TestDataFiles\security_newUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE658C6-78D6-4A01-A191-3A294C92FD04}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B30C873-E4AB-4AE4-A1BA-CDCF4E7252E3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -791,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:C42"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>